<commit_message>
Hints and fixes added
and change in historized reference table
</commit_message>
<xml_diff>
--- a/Kategorie Termintreue.xlsx
+++ b/Kategorie Termintreue.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://m2datade-my.sharepoint.com/personal/michael_m2data_de/Documents/Dokumente/GitHub/Samen und Pflanzen Willibald - DWH Beispiel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://m2datade-my.sharepoint.com/personal/michael_m2data_de/Documents/Dokumente/GitHub/Willibald-Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="31" documentId="8_{8EB9BD76-3C76-4484-A22D-AE4FA1A682EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2AA45E92-04DA-4BB9-B17E-32B38F5344B8}"/>
+  <xr:revisionPtr revIDLastSave="32" documentId="8_{8EB9BD76-3C76-4484-A22D-AE4FA1A682EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{93D214C6-7AB3-4E9A-B07F-BE99B6B90EBB}"/>
   <bookViews>
-    <workbookView xWindow="6948" yWindow="840" windowWidth="38016" windowHeight="20700" xr2:uid="{82133E7D-31B6-4AF3-BF13-A032A0378FCE}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="25536" xr2:uid="{82133E7D-31B6-4AF3-BF13-A032A0378FCE}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="29">
   <si>
     <t>Bezeichnung</t>
   </si>
@@ -120,6 +120,9 @@
   </si>
   <si>
     <t>bis zu 10 Tage zu spät</t>
+  </si>
+  <si>
+    <t>deutlich zu früh</t>
   </si>
 </sst>
 </file>
@@ -172,6 +175,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -474,7 +481,7 @@
   <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16:D25"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -660,7 +667,7 @@
         <v>26</v>
       </c>
       <c r="D18" t="s">
-        <v>4</v>
+        <v>28</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
added additonal entries in historized reftable
</commit_message>
<xml_diff>
--- a/Kategorie Termintreue.xlsx
+++ b/Kategorie Termintreue.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://m2datade-my.sharepoint.com/personal/michael_m2data_de/Documents/Dokumente/GitHub/Willibald-Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="32" documentId="8_{8EB9BD76-3C76-4484-A22D-AE4FA1A682EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{93D214C6-7AB3-4E9A-B07F-BE99B6B90EBB}"/>
+  <xr:revisionPtr revIDLastSave="37" documentId="8_{8EB9BD76-3C76-4484-A22D-AE4FA1A682EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E0C6192E-827B-4E12-92E0-6C72173D8578}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="25536" xr2:uid="{82133E7D-31B6-4AF3-BF13-A032A0378FCE}"/>
+    <workbookView xWindow="8844" yWindow="1908" windowWidth="34560" windowHeight="18684" xr2:uid="{82133E7D-31B6-4AF3-BF13-A032A0378FCE}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="32">
   <si>
     <t>Bezeichnung</t>
   </si>
@@ -123,6 +123,15 @@
   </si>
   <si>
     <t>deutlich zu früh</t>
+  </si>
+  <si>
+    <t>yyy</t>
+  </si>
+  <si>
+    <t>noch nicht geliefert</t>
+  </si>
+  <si>
+    <t>noch nicht relevant</t>
   </si>
 </sst>
 </file>
@@ -175,10 +184,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -478,10 +483,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7DF148F-D7BD-4F1A-AE1B-DE579DB5CF77}">
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -623,152 +628,181 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
         <v>2</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B19" t="s">
         <v>3</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C19" t="s">
         <v>0</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D19" t="s">
         <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17">
-        <v>-1000000</v>
-      </c>
-      <c r="B17">
-        <v>-10</v>
-      </c>
-      <c r="C17" t="s">
-        <v>24</v>
-      </c>
-      <c r="D17" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18">
-        <v>-10</v>
-      </c>
-      <c r="B18">
-        <v>-4</v>
-      </c>
-      <c r="C18" t="s">
-        <v>26</v>
-      </c>
-      <c r="D18" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19">
-        <v>-4</v>
-      </c>
-      <c r="B19">
-        <v>-1</v>
-      </c>
-      <c r="C19" t="s">
-        <v>25</v>
-      </c>
-      <c r="D19" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20">
-        <v>-1</v>
+        <v>-1000000</v>
       </c>
       <c r="B20">
-        <v>1</v>
+        <v>-10</v>
       </c>
       <c r="C20" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="D20" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21">
-        <v>1</v>
+        <v>-10</v>
       </c>
       <c r="B21">
-        <v>4</v>
+        <v>-4</v>
       </c>
       <c r="C21" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="D21" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22">
+        <v>-4</v>
+      </c>
+      <c r="B22">
+        <v>-1</v>
+      </c>
+      <c r="C22" t="s">
+        <v>25</v>
+      </c>
+      <c r="D22" t="s">
         <v>4</v>
-      </c>
-      <c r="B22">
-        <v>10</v>
-      </c>
-      <c r="C22" t="s">
-        <v>27</v>
-      </c>
-      <c r="D22" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23">
+        <v>-1</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23" t="s">
+        <v>7</v>
+      </c>
+      <c r="D23" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>1</v>
+      </c>
+      <c r="B24">
+        <v>4</v>
+      </c>
+      <c r="C24" t="s">
+        <v>8</v>
+      </c>
+      <c r="D24" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>4</v>
+      </c>
+      <c r="B25">
         <v>10</v>
       </c>
-      <c r="B23">
+      <c r="C25" t="s">
+        <v>27</v>
+      </c>
+      <c r="D25" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>10</v>
+      </c>
+      <c r="B26">
         <v>1000000</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C26" t="s">
         <v>10</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D26" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
         <v>15</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B27" t="s">
         <v>16</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C27" t="s">
         <v>17</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D27" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
         <v>21</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B28" t="s">
         <v>21</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C28" t="s">
         <v>22</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D28" t="s">
         <v>23</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>29</v>
+      </c>
+      <c r="B29" t="s">
+        <v>29</v>
+      </c>
+      <c r="C29" t="s">
+        <v>30</v>
+      </c>
+      <c r="D29" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>